<commit_message>
Anh doc qua nhe
</commit_message>
<xml_diff>
--- a/GreenEffect.Server/Database/Cau truc database.xlsx
+++ b/GreenEffect.Server/Database/Cau truc database.xlsx
@@ -4,18 +4,167 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="Customers" sheetId="3" r:id="rId3"/>
+    <sheet name="CustomersLocation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Op</t>
+  </si>
+  <si>
+    <t>IdenUser</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Nếu OP = 0 thì Sau khi đăng nhập sẽ vào giao diện chính, Op=1 Thì sau khi đăng nhập sẽ ra bảng lọc khách hàng. Sau khi lọc khách hàng xong thì chọn vào 1 khách hàng  sẽ lưu lại tọa độ và vào giao diện chính(tất cả các chức năng phía sau sẽ ăn theo khách hàng vừa chọn)</t>
+  </si>
+  <si>
+    <t>Chứa Identity ngầm của phần mềm</t>
+  </si>
+  <si>
+    <t>CustomersId</t>
+  </si>
+  <si>
+    <t>CustomersName</t>
+  </si>
+  <si>
+    <t>nvarchar(100)</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>nvarhar(200)</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>nvarchar(30)</t>
+  </si>
+  <si>
+    <t>IdenCustomers</t>
+  </si>
+  <si>
+    <t>Kiểu dữ liệu</t>
+  </si>
+  <si>
+    <t>Các trường</t>
+  </si>
+  <si>
+    <t>Chứa mã khách hàng</t>
+  </si>
+  <si>
+    <t>Chứa tên khách hàng</t>
+  </si>
+  <si>
+    <t>Địa chỉ khách hàng</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Chứa Identity của phần mềm tương ứng với bảng khách hàng</t>
+  </si>
+  <si>
+    <t>Chứa Identity của phần mềm tương ứng với bảng User</t>
+  </si>
+  <si>
+    <t>LocationName</t>
+  </si>
+  <si>
+    <t>nvarchar(500)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>nvarchar(200)</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>IdenCustomersLocation</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>Chứa Identity của bảng khách hàng</t>
+  </si>
+  <si>
+    <t>Chứa tên địa điểm</t>
+  </si>
+  <si>
+    <t>Chứa Nội dung địa điểm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chứa kinh độ </t>
+  </si>
+  <si>
+    <t>Chứa vĩ độ</t>
+  </si>
+  <si>
+    <t>Chứa identity của bảng user (iden phần mềm)</t>
+  </si>
+  <si>
+    <t>Chứa iden để đồng bộ</t>
+  </si>
+  <si>
+    <t>nếu =1 ko hiển thị</t>
+  </si>
+  <si>
+    <t>Haithanh#1</t>
+  </si>
+  <si>
+    <t>TTDH</t>
+  </si>
+  <si>
+    <t>1+2=3</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,13 +180,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -53,9 +223,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3392,7 +3570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
@@ -3408,4 +3586,347 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="86.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="39.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>